<commit_message>
50 sentences added.if can add some sentences pleas add them
</commit_message>
<xml_diff>
--- a/V.P.V.AverANNA/eng-sentences.xlsx
+++ b/V.P.V.AverANNA/eng-sentences.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="88">
   <si>
     <t xml:space="preserve">Who are your favorite performers or bands?</t>
   </si>
@@ -167,6 +167,123 @@
   </si>
   <si>
     <t xml:space="preserve">Please write it down.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">I need to go now.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">I feel good.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Thank you very much.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Thanks for your help.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Be careful.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">I'd like to go home.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">I love you.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">I give up.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">This doesn't work.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">They'll be right back.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">I'm bored.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Take it outside.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Please speak slower.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">If you need my help, please let me know.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">I'm happy.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">I'm going there next year.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">I'm cold.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Thank you miss.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Everything is ready.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">That looks old.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Good afternoon.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Hurry!</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Take your time.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">I don't mind.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">That's a good school.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">I have one in my car.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">I'll come back later.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tell him that I need to talk to him.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">I've never seen that before.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">You're very smart.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">These books are ours.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Come here.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">I've already seen it.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">I'm just looking.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Thanks for everything.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">I'd like to use the internet</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Here it is.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Happy Birthday.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">I'm getting ready to go out.</t>
   </si>
 </sst>
 </file>
@@ -181,6 +298,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -201,6 +319,7 @@
       <sz val="10"/>
       <name val="Courier New"/>
       <family val="3"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -271,16 +390,16 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:B50"/>
+  <dimension ref="A1:B100"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A24" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A50" activeCellId="0" sqref="A50"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A74" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A100" activeCellId="0" sqref="A100"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="112.54"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="23.89"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="23.88"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="3" style="0" width="11.52"/>
   </cols>
   <sheetData>
@@ -534,6 +653,256 @@
     <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="0" t="s">
         <v>48</v>
+      </c>
+    </row>
+    <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A51" s="0" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A52" s="0" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="53" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A53" s="0" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="54" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A54" s="0" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="55" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A55" s="0" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="56" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A56" s="0" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="57" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A57" s="0" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="58" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A58" s="0" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="59" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A59" s="0" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="60" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A60" s="0" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="61" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A61" s="0" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="62" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A62" s="0" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="63" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A63" s="0" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="64" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A64" s="0" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="65" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A65" s="0" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="66" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A66" s="0" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="67" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A67" s="0" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="68" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A68" s="0" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="69" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A69" s="0" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="70" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A70" s="0" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="71" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A71" s="0" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="72" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A72" s="0" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="73" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A73" s="0" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="74" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A74" s="0" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="75" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A75" s="0" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="76" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A76" s="0" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="77" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A77" s="0" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="78" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A78" s="0" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="79" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A79" s="0" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="80" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A80" s="0" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="81" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A81" s="0" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="82" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A82" s="0" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="83" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A83" s="0" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="84" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A84" s="0" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="85" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A85" s="0" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="86" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A86" s="0" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="87" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A87" s="0" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="88" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A88" s="0" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="89" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A89" s="0" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="90" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A90" s="0" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="91" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A91" s="0" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="92" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A92" s="0" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="93" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A93" s="0" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="94" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A94" s="0" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="95" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A95" s="0" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="96" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A96" s="0" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="97" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A97" s="0" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="98" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A98" s="0" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="99" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A99" s="0" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="100" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A100" s="0" t="s">
+        <v>50</v>
       </c>
     </row>
   </sheetData>

</xml_diff>